<commit_message>
Got Q_learning to work by adding artificial damping. Deleted some files.
</commit_message>
<xml_diff>
--- a/Working/qmotion_EXAMPLE_OUTPUT.xlsx
+++ b/Working/qmotion_EXAMPLE_OUTPUT.xlsx
@@ -22,10 +22,10 @@
     <t>It gets the occasional application of negative torque -0.03 to keep it there.</t>
   </si>
   <si>
-    <t>The pendulum, after many oscillations, has built up enough momentum to swing counter-clockwis past an almost straight up angle, about 1.69 radians.</t>
+    <t>N.B. The output file of the program is qmotion.txt, *not* an Excel file.</t>
   </si>
   <si>
-    <t>N.B. The output file of the program is qmotion.txt, *not* an Excel file.</t>
+    <t>The pendulum, after many oscillations, has built up enough momentum to swing counter-clockwise past a straight up angle, 1.5708 radians, to about 1.69 radians.</t>
   </si>
 </sst>
 </file>
@@ -12614,11 +12614,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137495296"/>
-        <c:axId val="137496832"/>
+        <c:axId val="158279168"/>
+        <c:axId val="158281088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="137495296"/>
+        <c:axId val="158279168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12627,7 +12627,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137496832"/>
+        <c:crossAx val="158281088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12635,7 +12635,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137496832"/>
+        <c:axId val="158281088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12646,7 +12646,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137495296"/>
+        <c:crossAx val="158279168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12993,7 +12993,7 @@
   <dimension ref="A1:I4000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13477,7 +13477,7 @@
         <v>-289.10599999999999</v>
       </c>
       <c r="I28" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -13534,7 +13534,7 @@
         <v>-298.83100000000002</v>
       </c>
       <c r="I31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>